<commit_message>
ADD TABLE `users`   ADD PRIMARY KEY (`id`);
--
-- AUTO_INCREMENT for dumped tables
</commit_message>
<xml_diff>
--- a/ادارة البحث.xlsx
+++ b/ادارة البحث.xlsx
@@ -384,6 +384,194 @@
     </font>
     <font>
       <sz val="20"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="18"/>
       <b/>
     </font>
     <font>
@@ -1614,6 +1802,53 @@
     <fill/>
     <fill/>
     <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="D9D9D9"/>
@@ -3363,6 +3598,335 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3384,7 +3948,7 @@
     <xf fontId="5" fillId="6" borderId="5" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="6" fillId="7" borderId="6" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="6" fillId="7" borderId="6" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="7" fillId="8" borderId="7" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3402,7 +3966,7 @@
     <xf fontId="11" fillId="12" borderId="11" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="12" fillId="13" borderId="12" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="12" fillId="13" borderId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="13" fillId="14" borderId="13" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3420,7 +3984,7 @@
     <xf fontId="17" fillId="18" borderId="17" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="18" fillId="19" borderId="18" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="18" fillId="19" borderId="18" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="19" fillId="20" borderId="19" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3438,7 +4002,7 @@
     <xf fontId="23" fillId="24" borderId="23" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="24" fillId="25" borderId="24" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="24" fillId="25" borderId="24" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="25" fillId="26" borderId="25" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3456,7 +4020,7 @@
     <xf fontId="29" fillId="30" borderId="29" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="30" fillId="31" borderId="30" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="30" fillId="31" borderId="30" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="31" fillId="32" borderId="31" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3474,7 +4038,7 @@
     <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3492,7 +4056,7 @@
     <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3510,7 +4074,7 @@
     <xf fontId="47" fillId="48" borderId="47" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="48" fillId="49" borderId="48" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="48" fillId="49" borderId="48" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="49" fillId="50" borderId="49" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3528,7 +4092,7 @@
     <xf fontId="53" fillId="54" borderId="53" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="54" fillId="55" borderId="54" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="54" fillId="55" borderId="54" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="55" fillId="56" borderId="55" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3546,7 +4110,7 @@
     <xf fontId="59" fillId="60" borderId="59" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="60" fillId="61" borderId="60" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="60" fillId="61" borderId="60" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="61" fillId="62" borderId="61" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3564,7 +4128,7 @@
     <xf fontId="65" fillId="66" borderId="65" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="66" fillId="67" borderId="66" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="66" fillId="67" borderId="66" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="67" fillId="68" borderId="67" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3582,7 +4146,7 @@
     <xf fontId="71" fillId="72" borderId="71" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="72" fillId="73" borderId="72" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="72" fillId="73" borderId="72" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="73" fillId="74" borderId="73" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3600,7 +4164,7 @@
     <xf fontId="77" fillId="78" borderId="77" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="78" fillId="79" borderId="78" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="78" fillId="79" borderId="78" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="79" fillId="80" borderId="79" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3618,7 +4182,7 @@
     <xf fontId="83" fillId="84" borderId="83" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="84" fillId="85" borderId="84" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="84" fillId="85" borderId="84" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="85" fillId="86" borderId="85" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3636,7 +4200,7 @@
     <xf fontId="89" fillId="90" borderId="89" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="90" fillId="91" borderId="90" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="90" fillId="91" borderId="90" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="91" fillId="92" borderId="91" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3654,7 +4218,7 @@
     <xf fontId="95" fillId="96" borderId="95" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="96" fillId="97" borderId="96" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="96" fillId="97" borderId="96" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="97" fillId="98" borderId="97" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3672,7 +4236,7 @@
     <xf fontId="101" fillId="102" borderId="101" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="102" fillId="103" borderId="102" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="102" fillId="103" borderId="102" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="103" fillId="104" borderId="103" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3690,7 +4254,7 @@
     <xf fontId="107" fillId="108" borderId="107" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="108" fillId="109" borderId="108" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="108" fillId="109" borderId="108" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="109" fillId="110" borderId="109" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3708,7 +4272,7 @@
     <xf fontId="113" fillId="114" borderId="113" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="114" fillId="115" borderId="114" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="114" fillId="115" borderId="114" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="115" fillId="116" borderId="115" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3726,7 +4290,7 @@
     <xf fontId="119" fillId="120" borderId="119" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="120" fillId="121" borderId="120" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="120" fillId="121" borderId="120" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="121" fillId="122" borderId="121" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3744,7 +4308,7 @@
     <xf fontId="125" fillId="126" borderId="125" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="126" fillId="127" borderId="126" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="126" fillId="127" borderId="126" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="127" fillId="128" borderId="127" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3762,7 +4326,7 @@
     <xf fontId="131" fillId="132" borderId="131" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="132" fillId="133" borderId="132" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="132" fillId="133" borderId="132" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="133" fillId="134" borderId="133" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3780,7 +4344,7 @@
     <xf fontId="137" fillId="138" borderId="137" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="138" fillId="139" borderId="138" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="138" fillId="139" borderId="138" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="139" fillId="140" borderId="139" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3798,7 +4362,7 @@
     <xf fontId="143" fillId="144" borderId="143" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="144" fillId="145" borderId="144" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="144" fillId="145" borderId="144" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="145" fillId="146" borderId="145" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3816,7 +4380,7 @@
     <xf fontId="149" fillId="150" borderId="149" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="150" fillId="151" borderId="150" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="150" fillId="151" borderId="150" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="151" fillId="152" borderId="151" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3834,7 +4398,7 @@
     <xf fontId="155" fillId="156" borderId="155" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="156" fillId="157" borderId="156" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="156" fillId="157" borderId="156" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="157" fillId="158" borderId="157" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3852,7 +4416,7 @@
     <xf fontId="161" fillId="162" borderId="161" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="162" fillId="163" borderId="162" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="162" fillId="163" borderId="162" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="163" fillId="164" borderId="163" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3870,7 +4434,7 @@
     <xf fontId="167" fillId="168" borderId="167" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="168" fillId="169" borderId="168" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="168" fillId="169" borderId="168" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="169" fillId="170" borderId="169" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3888,7 +4452,7 @@
     <xf fontId="173" fillId="174" borderId="173" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="174" fillId="175" borderId="174" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="174" fillId="175" borderId="174" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="175" fillId="176" borderId="175" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3906,7 +4470,7 @@
     <xf fontId="179" fillId="180" borderId="179" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="180" fillId="181" borderId="180" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="180" fillId="181" borderId="180" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="181" fillId="182" borderId="181" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3924,7 +4488,7 @@
     <xf fontId="185" fillId="186" borderId="185" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="186" fillId="187" borderId="186" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="186" fillId="187" borderId="186" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="187" fillId="188" borderId="187" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3942,7 +4506,7 @@
     <xf fontId="191" fillId="192" borderId="191" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="192" fillId="193" borderId="192" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="192" fillId="193" borderId="192" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="193" fillId="194" borderId="193" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3960,7 +4524,7 @@
     <xf fontId="197" fillId="198" borderId="197" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="198" fillId="199" borderId="198" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="198" fillId="199" borderId="198" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="199" fillId="200" borderId="199" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3978,7 +4542,7 @@
     <xf fontId="203" fillId="204" borderId="203" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="204" fillId="205" borderId="204" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="204" fillId="205" borderId="204" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="205" fillId="206" borderId="205" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -3996,7 +4560,7 @@
     <xf fontId="209" fillId="210" borderId="209" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="210" fillId="211" borderId="210" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="210" fillId="211" borderId="210" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="211" fillId="212" borderId="211" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -4014,7 +4578,7 @@
     <xf fontId="215" fillId="216" borderId="215" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="216" fillId="217" borderId="216" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="216" fillId="217" borderId="216" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="217" fillId="218" borderId="217" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -4032,7 +4596,7 @@
     <xf fontId="221" fillId="222" borderId="221" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="222" fillId="223" borderId="222" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="222" fillId="223" borderId="222" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="223" fillId="224" borderId="223" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -4050,7 +4614,7 @@
     <xf fontId="227" fillId="228" borderId="227" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="228" fillId="229" borderId="228" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="228" fillId="229" borderId="228" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="229" fillId="230" borderId="229" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -4068,7 +4632,7 @@
     <xf fontId="233" fillId="234" borderId="233" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="234" fillId="235" borderId="234" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+    <xf fontId="234" fillId="235" borderId="234" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf fontId="235" fillId="236" borderId="235" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
@@ -4086,22 +4650,163 @@
     <xf fontId="239" fillId="240" borderId="239" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf fontId="240" fillId="241" borderId="240" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf fontId="241" fillId="242" borderId="241" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf fontId="242" fillId="243" borderId="242" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf fontId="243" fillId="244" borderId="243" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf fontId="244" fillId="245" borderId="244" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf fontId="245" fillId="246" borderId="245" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="240" fillId="241" borderId="240" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="241" fillId="242" borderId="241" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="242" fillId="243" borderId="242" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="243" fillId="244" borderId="243" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="244" fillId="245" borderId="244" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="245" fillId="246" borderId="245" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="246" fillId="247" borderId="246" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="247" fillId="248" borderId="247" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="248" fillId="249" borderId="248" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="249" fillId="250" borderId="249" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="250" fillId="251" borderId="250" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="251" fillId="252" borderId="251" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="252" fillId="253" borderId="252" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="253" fillId="254" borderId="253" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="254" fillId="255" borderId="254" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="255" fillId="256" borderId="255" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="256" fillId="257" borderId="256" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="257" fillId="258" borderId="257" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="258" fillId="259" borderId="258" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="259" fillId="260" borderId="259" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="260" fillId="261" borderId="260" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="261" fillId="262" borderId="261" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="262" fillId="263" borderId="262" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="263" fillId="264" borderId="263" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="264" fillId="265" borderId="264" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="265" fillId="266" borderId="265" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="266" fillId="267" borderId="266" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="267" fillId="268" borderId="267" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="268" fillId="269" borderId="268" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="269" fillId="270" borderId="269" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="270" fillId="271" borderId="270" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="271" fillId="272" borderId="271" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="272" fillId="273" borderId="272" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="273" fillId="274" borderId="273" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="274" fillId="275" borderId="274" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="275" fillId="276" borderId="275" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="276" fillId="277" borderId="276" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="277" fillId="278" borderId="277" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="278" fillId="279" borderId="278" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="279" fillId="280" borderId="279" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="280" fillId="281" borderId="280" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="281" fillId="282" borderId="281" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="282" fillId="283" borderId="282" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="283" fillId="284" borderId="283" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="284" fillId="285" borderId="284" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="285" fillId="286" borderId="285" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="286" fillId="287" borderId="286" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="287" fillId="288" borderId="287" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="288" fillId="289" borderId="288" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="289" fillId="290" borderId="289" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="290" fillId="291" borderId="290" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="291" fillId="292" borderId="291" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf fontId="292" fillId="293" borderId="292" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -4390,844 +5095,985 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="B1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="C1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="D1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="4">
+      <c r="E1" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="5">
+      <c r="F1" t="s" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="6">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="C2" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="D2" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="9">
+      <c r="E2" t="s" s="10">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="10">
+      <c r="F2" t="s" s="11">
         <v>9</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="11">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="12">
+      <c r="C3" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="C3" t="s" s="13">
+      <c r="D3" t="s" s="15">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="14">
+      <c r="E3" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="E3" t="s" s="15">
+      <c r="F3" t="s" s="17">
         <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="16">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="19">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="17">
+      <c r="C4" t="s" s="20">
         <v>14</v>
       </c>
-      <c r="C4" t="s" s="18">
+      <c r="D4" t="s" s="21">
         <v>7</v>
       </c>
-      <c r="D4" t="s" s="19">
+      <c r="E4" t="s" s="22">
         <v>8</v>
       </c>
-      <c r="E4" t="s" s="20">
+      <c r="F4" t="s" s="23">
         <v>9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="21">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="25">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="22">
+      <c r="C5" t="s" s="26">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="23">
+      <c r="D5" t="s" s="27">
         <v>7</v>
       </c>
-      <c r="D5" t="s" s="24">
+      <c r="E5" t="s" s="28">
         <v>8</v>
       </c>
-      <c r="E5" t="s" s="25">
+      <c r="F5" t="s" s="29">
         <v>9</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="26">
+      <c r="A6" s="30">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="31">
         <v>17</v>
       </c>
-      <c r="B6" t="s" s="27">
+      <c r="C6" t="s" s="32">
         <v>18</v>
       </c>
-      <c r="C6" t="s" s="28">
+      <c r="D6" t="s" s="33">
         <v>7</v>
       </c>
-      <c r="D6" t="s" s="29">
+      <c r="E6" t="s" s="34">
         <v>8</v>
       </c>
-      <c r="E6" t="s" s="30">
+      <c r="F6" t="s" s="35">
         <v>9</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="31">
+      <c r="A7" s="36">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="37">
         <v>19</v>
       </c>
-      <c r="B7" t="s" s="32">
+      <c r="C7" t="s" s="38">
         <v>20</v>
       </c>
-      <c r="C7" t="s" s="33">
+      <c r="D7" t="s" s="39">
         <v>7</v>
       </c>
-      <c r="D7" t="s" s="34">
+      <c r="E7" t="s" s="40">
         <v>8</v>
       </c>
-      <c r="E7" t="s" s="35">
+      <c r="F7" t="s" s="41">
         <v>9</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="36">
+      <c r="A8" s="42">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="43">
         <v>21</v>
       </c>
-      <c r="B8" t="s" s="37">
+      <c r="C8" t="s" s="44">
         <v>22</v>
       </c>
-      <c r="C8" t="s" s="38">
+      <c r="D8" t="s" s="45">
         <v>7</v>
       </c>
-      <c r="D8" t="s" s="39">
+      <c r="E8" t="s" s="46">
         <v>23</v>
       </c>
-      <c r="E8" t="s" s="40">
+      <c r="F8" t="s" s="47">
         <v>9</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="41">
+      <c r="A9" s="48">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="49">
         <v>24</v>
       </c>
-      <c r="B9" t="s" s="42">
+      <c r="C9" t="s" s="50">
         <v>25</v>
       </c>
-      <c r="C9" t="s" s="43">
+      <c r="D9" t="s" s="51">
         <v>7</v>
       </c>
-      <c r="D9" t="s" s="44">
+      <c r="E9" t="s" s="52">
         <v>8</v>
       </c>
-      <c r="E9" t="s" s="45">
+      <c r="F9" t="s" s="53">
         <v>9</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="46">
+      <c r="A10" s="54">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s" s="55">
         <v>26</v>
       </c>
-      <c r="B10" t="s" s="47">
+      <c r="C10" t="s" s="56">
         <v>27</v>
       </c>
-      <c r="C10" t="s" s="48">
+      <c r="D10" t="s" s="57">
         <v>7</v>
       </c>
-      <c r="D10" t="s" s="49">
+      <c r="E10" t="s" s="58">
         <v>8</v>
       </c>
-      <c r="E10" t="s" s="50">
+      <c r="F10" t="s" s="59">
         <v>9</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="51">
+      <c r="A11" s="60">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s" s="61">
         <v>28</v>
       </c>
-      <c r="B11" t="s" s="52">
+      <c r="C11" t="s" s="62">
         <v>29</v>
       </c>
-      <c r="C11" t="s" s="53">
+      <c r="D11" t="s" s="63">
         <v>7</v>
       </c>
-      <c r="D11" t="s" s="54">
+      <c r="E11" t="s" s="64">
         <v>23</v>
       </c>
-      <c r="E11" t="s" s="55">
+      <c r="F11" t="s" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s" s="56">
+      <c r="A12" s="66">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="67">
         <v>30</v>
       </c>
-      <c r="B12" t="s" s="57">
+      <c r="C12" t="s" s="68">
         <v>31</v>
       </c>
-      <c r="C12" t="s" s="58">
+      <c r="D12" t="s" s="69">
         <v>7</v>
       </c>
-      <c r="D12" t="s" s="59">
+      <c r="E12" t="s" s="70">
         <v>8</v>
       </c>
-      <c r="E12" t="s" s="60">
+      <c r="F12" t="s" s="71">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="61">
+      <c r="A13" s="72">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s" s="73">
         <v>32</v>
       </c>
-      <c r="B13" t="s" s="62">
+      <c r="C13" t="s" s="74">
         <v>33</v>
       </c>
-      <c r="C13" t="s" s="63">
+      <c r="D13" t="s" s="75">
         <v>7</v>
       </c>
-      <c r="D13" t="s" s="64">
+      <c r="E13" t="s" s="76">
         <v>23</v>
       </c>
-      <c r="E13" t="s" s="65">
+      <c r="F13" t="s" s="77">
         <v>9</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="66">
+      <c r="A14" s="78">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s" s="79">
         <v>34</v>
       </c>
-      <c r="B14" t="s" s="67">
+      <c r="C14" t="s" s="80">
         <v>35</v>
       </c>
-      <c r="C14" t="s" s="68">
+      <c r="D14" t="s" s="81">
         <v>7</v>
       </c>
-      <c r="D14" t="s" s="69">
+      <c r="E14" t="s" s="82">
         <v>8</v>
       </c>
-      <c r="E14" t="s" s="70">
+      <c r="F14" t="s" s="83">
         <v>9</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="71">
+      <c r="A15" s="84">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s" s="85">
         <v>36</v>
       </c>
-      <c r="B15" t="s" s="72">
+      <c r="C15" t="s" s="86">
         <v>37</v>
       </c>
-      <c r="C15" t="s" s="73">
+      <c r="D15" t="s" s="87">
         <v>7</v>
       </c>
-      <c r="D15" t="s" s="74">
+      <c r="E15" t="s" s="88">
         <v>8</v>
       </c>
-      <c r="E15" t="s" s="75">
+      <c r="F15" t="s" s="89">
         <v>9</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s" s="76">
+      <c r="A16" s="90">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s" s="91">
         <v>38</v>
       </c>
-      <c r="B16" t="s" s="77">
+      <c r="C16" t="s" s="92">
         <v>39</v>
       </c>
-      <c r="C16" t="s" s="78">
+      <c r="D16" t="s" s="93">
         <v>7</v>
       </c>
-      <c r="D16" t="s" s="79">
+      <c r="E16" t="s" s="94">
         <v>8</v>
       </c>
-      <c r="E16" t="s" s="80">
+      <c r="F16" t="s" s="95">
         <v>9</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="81">
+      <c r="A17" s="96">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s" s="97">
         <v>40</v>
       </c>
-      <c r="B17" t="s" s="82">
+      <c r="C17" t="s" s="98">
         <v>41</v>
       </c>
-      <c r="C17" t="s" s="83">
+      <c r="D17" t="s" s="99">
         <v>7</v>
       </c>
-      <c r="D17" t="s" s="84">
+      <c r="E17" t="s" s="100">
         <v>23</v>
       </c>
-      <c r="E17" t="s" s="85">
+      <c r="F17" t="s" s="101">
         <v>9</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="86">
+      <c r="A18" s="102">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s" s="103">
         <v>42</v>
       </c>
-      <c r="B18" t="s" s="87">
+      <c r="C18" t="s" s="104">
         <v>43</v>
       </c>
-      <c r="C18" t="s" s="88">
+      <c r="D18" t="s" s="105">
         <v>7</v>
       </c>
-      <c r="D18" t="s" s="89">
+      <c r="E18" t="s" s="106">
         <v>8</v>
       </c>
-      <c r="E18" t="s" s="90">
+      <c r="F18" t="s" s="107">
         <v>9</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="91">
+      <c r="A19" s="108">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s" s="109">
         <v>44</v>
       </c>
-      <c r="B19" t="s" s="92">
+      <c r="C19" t="s" s="110">
         <v>45</v>
       </c>
-      <c r="C19" t="s" s="93">
+      <c r="D19" t="s" s="111">
         <v>7</v>
       </c>
-      <c r="D19" t="s" s="94">
+      <c r="E19" t="s" s="112">
         <v>23</v>
       </c>
-      <c r="E19" t="s" s="95">
+      <c r="F19" t="s" s="113">
         <v>9</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="96">
+      <c r="A20" s="114">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="115">
         <v>46</v>
       </c>
-      <c r="B20" t="s" s="97">
+      <c r="C20" t="s" s="116">
         <v>47</v>
       </c>
-      <c r="C20" t="s" s="98">
+      <c r="D20" t="s" s="117">
         <v>7</v>
       </c>
-      <c r="D20" t="s" s="99">
+      <c r="E20" t="s" s="118">
         <v>23</v>
       </c>
-      <c r="E20" t="s" s="100">
+      <c r="F20" t="s" s="119">
         <v>9</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s" s="101">
+      <c r="A21" s="120">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="121">
         <v>48</v>
       </c>
-      <c r="B21" t="s" s="102">
+      <c r="C21" t="s" s="122">
         <v>49</v>
       </c>
-      <c r="C21" t="s" s="103">
+      <c r="D21" t="s" s="123">
         <v>7</v>
       </c>
-      <c r="D21" t="s" s="104">
+      <c r="E21" t="s" s="124">
         <v>8</v>
       </c>
-      <c r="E21" t="s" s="105">
+      <c r="F21" t="s" s="125">
         <v>9</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="106">
+      <c r="A22" s="126">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s" s="127">
         <v>50</v>
       </c>
-      <c r="B22" t="s" s="107">
+      <c r="C22" t="s" s="128">
         <v>51</v>
       </c>
-      <c r="C22" t="s" s="108">
+      <c r="D22" t="s" s="129">
         <v>7</v>
       </c>
-      <c r="D22" t="s" s="109">
+      <c r="E22" t="s" s="130">
         <v>52</v>
       </c>
-      <c r="E22" t="s" s="110">
+      <c r="F22" t="s" s="131">
         <v>9</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s" s="111">
+      <c r="A23" s="132">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s" s="133">
         <v>53</v>
       </c>
-      <c r="B23" t="s" s="112">
+      <c r="C23" t="s" s="134">
         <v>54</v>
       </c>
-      <c r="C23" t="s" s="113">
+      <c r="D23" t="s" s="135">
         <v>7</v>
       </c>
-      <c r="D23" t="s" s="114">
+      <c r="E23" t="s" s="136">
         <v>23</v>
       </c>
-      <c r="E23" t="s" s="115">
+      <c r="F23" t="s" s="137">
         <v>9</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="116">
+      <c r="A24" s="138">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s" s="139">
         <v>55</v>
       </c>
-      <c r="B24" t="s" s="117">
+      <c r="C24" t="s" s="140">
         <v>56</v>
       </c>
-      <c r="C24" t="s" s="118">
+      <c r="D24" t="s" s="141">
         <v>7</v>
       </c>
-      <c r="D24" t="s" s="119">
+      <c r="E24" t="s" s="142">
         <v>23</v>
       </c>
-      <c r="E24" t="s" s="120">
+      <c r="F24" t="s" s="143">
         <v>9</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="121">
+      <c r="A25" s="144">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s" s="145">
         <v>57</v>
       </c>
-      <c r="B25" t="s" s="122">
+      <c r="C25" t="s" s="146">
         <v>58</v>
       </c>
-      <c r="C25" t="s" s="123">
+      <c r="D25" t="s" s="147">
         <v>7</v>
       </c>
-      <c r="D25" t="s" s="124">
+      <c r="E25" t="s" s="148">
         <v>8</v>
       </c>
-      <c r="E25" t="s" s="125">
+      <c r="F25" t="s" s="149">
         <v>9</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="126">
+      <c r="A26" s="150">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s" s="151">
         <v>59</v>
       </c>
-      <c r="B26" t="s" s="127">
+      <c r="C26" t="s" s="152">
         <v>60</v>
       </c>
-      <c r="C26" t="s" s="128">
+      <c r="D26" t="s" s="153">
         <v>7</v>
       </c>
-      <c r="D26" t="s" s="129">
+      <c r="E26" t="s" s="154">
         <v>8</v>
       </c>
-      <c r="E26" t="s" s="130">
+      <c r="F26" t="s" s="155">
         <v>9</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="131">
+      <c r="A27" s="156">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s" s="157">
         <v>61</v>
       </c>
-      <c r="B27" t="s" s="132">
+      <c r="C27" t="s" s="158">
         <v>62</v>
       </c>
-      <c r="C27" t="s" s="133">
+      <c r="D27" t="s" s="159">
         <v>7</v>
       </c>
-      <c r="D27" t="s" s="134">
+      <c r="E27" t="s" s="160">
         <v>8</v>
       </c>
-      <c r="E27" t="s" s="135">
+      <c r="F27" t="s" s="161">
         <v>9</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s" s="136">
+      <c r="A28" s="162">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s" s="163">
         <v>63</v>
       </c>
-      <c r="B28" t="s" s="137">
+      <c r="C28" t="s" s="164">
         <v>64</v>
       </c>
-      <c r="C28" t="s" s="138">
+      <c r="D28" t="s" s="165">
         <v>7</v>
       </c>
-      <c r="D28" t="s" s="139">
+      <c r="E28" t="s" s="166">
         <v>8</v>
       </c>
-      <c r="E28" t="s" s="140">
+      <c r="F28" t="s" s="167">
         <v>9</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="141">
+      <c r="A29" s="168">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s" s="169">
         <v>65</v>
       </c>
-      <c r="B29" t="s" s="142">
+      <c r="C29" t="s" s="170">
         <v>66</v>
       </c>
-      <c r="C29" t="s" s="143">
+      <c r="D29" t="s" s="171">
         <v>7</v>
       </c>
-      <c r="D29" t="s" s="144">
+      <c r="E29" t="s" s="172">
         <v>8</v>
       </c>
-      <c r="E29" t="s" s="145">
+      <c r="F29" t="s" s="173">
         <v>9</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s" s="146">
+      <c r="A30" s="174">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s" s="175">
         <v>67</v>
       </c>
-      <c r="B30" t="s" s="147">
+      <c r="C30" t="s" s="176">
         <v>68</v>
       </c>
-      <c r="C30" t="s" s="148">
+      <c r="D30" t="s" s="177">
         <v>7</v>
       </c>
-      <c r="D30" t="s" s="149">
+      <c r="E30" t="s" s="178">
         <v>8</v>
       </c>
-      <c r="E30" t="s" s="150">
+      <c r="F30" t="s" s="179">
         <v>9</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s" s="151">
+      <c r="A31" s="180">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s" s="181">
         <v>69</v>
       </c>
-      <c r="B31" t="s" s="152">
+      <c r="C31" t="s" s="182">
         <v>70</v>
       </c>
-      <c r="C31" t="s" s="153">
+      <c r="D31" t="s" s="183">
         <v>7</v>
       </c>
-      <c r="D31" t="s" s="154">
+      <c r="E31" t="s" s="184">
         <v>71</v>
       </c>
-      <c r="E31" t="s" s="155">
+      <c r="F31" t="s" s="185">
         <v>9</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s" s="156">
+      <c r="A32" s="186">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s" s="187">
         <v>72</v>
       </c>
-      <c r="B32" t="s" s="157">
+      <c r="C32" t="s" s="188">
         <v>73</v>
       </c>
-      <c r="C32" t="s" s="158">
+      <c r="D32" t="s" s="189">
         <v>7</v>
       </c>
-      <c r="D32" t="s" s="159">
+      <c r="E32" t="s" s="190">
         <v>8</v>
       </c>
-      <c r="E32" t="s" s="160">
+      <c r="F32" t="s" s="191">
         <v>9</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s" s="161">
+      <c r="A33" s="192">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s" s="193">
         <v>74</v>
       </c>
-      <c r="B33" t="s" s="162">
+      <c r="C33" t="s" s="194">
         <v>75</v>
       </c>
-      <c r="C33" t="s" s="163">
+      <c r="D33" t="s" s="195">
         <v>7</v>
       </c>
-      <c r="D33" t="s" s="164">
+      <c r="E33" t="s" s="196">
         <v>8</v>
       </c>
-      <c r="E33" t="s" s="165">
+      <c r="F33" t="s" s="197">
         <v>9</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s" s="166">
+      <c r="A34" s="198">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s" s="199">
         <v>76</v>
       </c>
-      <c r="B34" t="s" s="167">
+      <c r="C34" t="s" s="200">
         <v>77</v>
       </c>
-      <c r="C34" t="s" s="168">
+      <c r="D34" t="s" s="201">
         <v>7</v>
       </c>
-      <c r="D34" t="s" s="169">
+      <c r="E34" t="s" s="202">
         <v>8</v>
       </c>
-      <c r="E34" t="s" s="170">
+      <c r="F34" t="s" s="203">
         <v>9</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s" s="171">
+      <c r="A35" s="204">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s" s="205">
         <v>78</v>
       </c>
-      <c r="B35" t="s" s="172">
+      <c r="C35" t="s" s="206">
         <v>79</v>
       </c>
-      <c r="C35" t="s" s="173">
+      <c r="D35" t="s" s="207">
         <v>7</v>
       </c>
-      <c r="D35" t="s" s="174">
+      <c r="E35" t="s" s="208">
         <v>8</v>
       </c>
-      <c r="E35" t="s" s="175">
+      <c r="F35" t="s" s="209">
         <v>9</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="176">
+      <c r="A36" s="210">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s" s="211">
         <v>80</v>
       </c>
-      <c r="B36" t="s" s="177">
+      <c r="C36" t="s" s="212">
         <v>81</v>
       </c>
-      <c r="C36" t="s" s="178">
+      <c r="D36" t="s" s="213">
         <v>7</v>
       </c>
-      <c r="D36" t="s" s="179">
+      <c r="E36" t="s" s="214">
         <v>8</v>
       </c>
-      <c r="E36" t="s" s="180">
+      <c r="F36" t="s" s="215">
         <v>9</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s" s="181">
+      <c r="A37" s="216">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s" s="217">
         <v>82</v>
       </c>
-      <c r="B37" t="s" s="182">
+      <c r="C37" t="s" s="218">
         <v>83</v>
       </c>
-      <c r="C37" t="s" s="183">
+      <c r="D37" t="s" s="219">
         <v>7</v>
       </c>
-      <c r="D37" t="s" s="184">
+      <c r="E37" t="s" s="220">
         <v>8</v>
       </c>
-      <c r="E37" t="s" s="185">
+      <c r="F37" t="s" s="221">
         <v>9</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s" s="186">
+      <c r="A38" s="222">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s" s="223">
         <v>84</v>
       </c>
-      <c r="B38" t="s" s="187">
+      <c r="C38" t="s" s="224">
         <v>85</v>
       </c>
-      <c r="C38" t="s" s="188">
+      <c r="D38" t="s" s="225">
         <v>7</v>
       </c>
-      <c r="D38" t="s" s="189">
+      <c r="E38" t="s" s="226">
         <v>23</v>
       </c>
-      <c r="E38" t="s" s="190">
+      <c r="F38" t="s" s="227">
         <v>9</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s" s="191">
+      <c r="A39" s="228">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s" s="229">
         <v>86</v>
       </c>
-      <c r="B39" t="s" s="192">
+      <c r="C39" t="s" s="230">
         <v>87</v>
       </c>
-      <c r="C39" t="s" s="193">
+      <c r="D39" t="s" s="231">
         <v>7</v>
       </c>
-      <c r="D39" t="s" s="194">
+      <c r="E39" t="s" s="232">
         <v>71</v>
       </c>
-      <c r="E39" t="s" s="195">
+      <c r="F39" t="s" s="233">
         <v>9</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s" s="196">
+      <c r="A40" s="234">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s" s="235">
         <v>88</v>
       </c>
-      <c r="B40" t="s" s="197">
+      <c r="C40" t="s" s="236">
         <v>89</v>
       </c>
-      <c r="C40" t="s" s="198">
+      <c r="D40" t="s" s="237">
         <v>7</v>
       </c>
-      <c r="D40" t="s" s="199">
+      <c r="E40" t="s" s="238">
         <v>8</v>
       </c>
-      <c r="E40" t="s" s="200">
+      <c r="F40" t="s" s="239">
         <v>9</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s" s="201">
+      <c r="A41" s="240">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s" s="241">
         <v>90</v>
       </c>
-      <c r="B41" t="s" s="202">
+      <c r="C41" t="s" s="242">
         <v>91</v>
       </c>
-      <c r="C41" t="s" s="203">
+      <c r="D41" t="s" s="243">
         <v>7</v>
       </c>
-      <c r="D41" t="s" s="204">
+      <c r="E41" t="s" s="244">
         <v>8</v>
       </c>
-      <c r="E41" t="s" s="205">
+      <c r="F41" t="s" s="245">
         <v>9</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s" s="206">
+      <c r="A42" s="246">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s" s="247">
         <v>92</v>
       </c>
-      <c r="B42" t="s" s="207">
+      <c r="C42" t="s" s="248">
         <v>93</v>
       </c>
-      <c r="C42" t="s" s="208">
+      <c r="D42" t="s" s="249">
         <v>7</v>
       </c>
-      <c r="D42" t="s" s="209">
+      <c r="E42" t="s" s="250">
         <v>8</v>
       </c>
-      <c r="E42" t="s" s="210">
+      <c r="F42" t="s" s="251">
         <v>9</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s" s="211">
+      <c r="A43" s="252">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s" s="253">
         <v>94</v>
       </c>
-      <c r="B43" t="s" s="212">
+      <c r="C43" t="s" s="254">
         <v>95</v>
       </c>
-      <c r="C43" t="s" s="213">
+      <c r="D43" t="s" s="255">
         <v>7</v>
       </c>
-      <c r="D43" t="s" s="214">
+      <c r="E43" t="s" s="256">
         <v>8</v>
       </c>
-      <c r="E43" t="s" s="215">
+      <c r="F43" t="s" s="257">
         <v>9</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s" s="216">
+      <c r="A44" s="258">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s" s="259">
         <v>96</v>
       </c>
-      <c r="B44" t="s" s="217">
+      <c r="C44" t="s" s="260">
         <v>97</v>
       </c>
-      <c r="C44" t="s" s="218">
+      <c r="D44" t="s" s="261">
         <v>7</v>
       </c>
-      <c r="D44" t="s" s="219">
+      <c r="E44" t="s" s="262">
         <v>8</v>
       </c>
-      <c r="E44" t="s" s="220">
+      <c r="F44" t="s" s="263">
         <v>9</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s" s="221">
+      <c r="A45" s="264">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s" s="265">
         <v>98</v>
       </c>
-      <c r="B45" t="s" s="222">
+      <c r="C45" t="s" s="266">
         <v>99</v>
       </c>
-      <c r="C45" t="s" s="223">
+      <c r="D45" t="s" s="267">
         <v>7</v>
       </c>
-      <c r="D45" t="s" s="224">
+      <c r="E45" t="s" s="268">
         <v>8</v>
       </c>
-      <c r="E45" t="s" s="225">
+      <c r="F45" t="s" s="269">
         <v>9</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s" s="226">
+      <c r="A46" s="270">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s" s="271">
         <v>100</v>
       </c>
-      <c r="B46" t="s" s="227">
+      <c r="C46" t="s" s="272">
         <v>101</v>
       </c>
-      <c r="C46" t="s" s="228">
+      <c r="D46" t="s" s="273">
         <v>7</v>
       </c>
-      <c r="D46" t="s" s="229">
+      <c r="E46" t="s" s="274">
         <v>8</v>
       </c>
-      <c r="E46" t="s" s="230">
+      <c r="F46" t="s" s="275">
         <v>9</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s" s="231">
+      <c r="A47" s="276">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s" s="277">
         <v>102</v>
       </c>
-      <c r="B47" t="s" s="232">
+      <c r="C47" t="s" s="278">
         <v>103</v>
       </c>
-      <c r="C47" t="s" s="233">
+      <c r="D47" t="s" s="279">
         <v>7</v>
       </c>
-      <c r="D47" t="s" s="234">
+      <c r="E47" t="s" s="280">
         <v>104</v>
       </c>
-      <c r="E47" t="s" s="235">
+      <c r="F47" t="s" s="281">
         <v>9</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s" s="236">
+      <c r="A48" s="282">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s" s="283">
         <v>105</v>
       </c>
-      <c r="B48" t="s" s="237">
+      <c r="C48" t="s" s="284">
         <v>106</v>
       </c>
-      <c r="C48" t="s" s="238">
+      <c r="D48" t="s" s="285">
         <v>7</v>
       </c>
-      <c r="D48" t="s" s="239">
+      <c r="E48" t="s" s="286">
         <v>23</v>
       </c>
-      <c r="E48" t="s" s="240">
+      <c r="F48" t="s" s="287">
         <v>9</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s" s="241">
+      <c r="B49" t="s" s="288">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s" s="289">
         <v>107</v>
       </c>
-      <c r="B49" t="s" s="242">
+      <c r="D49" t="s" s="290">
         <v>9</v>
       </c>
-      <c r="C49" t="s" s="243">
+      <c r="E49" t="s" s="291">
         <v>9</v>
       </c>
-      <c r="D49" t="s" s="244">
+      <c r="F49" t="s" s="292">
         <v>108</v>
-      </c>
-      <c r="E49" t="s" s="245">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>